<commit_message>
Simplificação da coluna benefícios
</commit_message>
<xml_diff>
--- a/job_info_gpt3_50.xlsx
+++ b/job_info_gpt3_50.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28004"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,23 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1226,7 +1242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1608,19 +1624,19 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="128.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="128.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1690,7 +1706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1725,7 +1741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1760,7 +1776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1795,7 +1811,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1830,7 +1846,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1865,7 +1881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1900,7 +1916,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -1935,7 +1951,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -1970,7 +1986,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -2040,7 +2056,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>108</v>
       </c>
@@ -2075,7 +2091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -2110,7 +2126,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -2145,7 +2161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -2180,7 +2196,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2215,7 +2231,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2250,7 +2266,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>157</v>
       </c>
@@ -2282,7 +2298,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -2317,7 +2333,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>157</v>
       </c>
@@ -2352,7 +2368,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -2387,7 +2403,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>157</v>
       </c>
@@ -2422,7 +2438,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -2457,7 +2473,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>157</v>
       </c>
@@ -2492,7 +2508,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>204</v>
       </c>
@@ -2527,7 +2543,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>214</v>
       </c>
@@ -2562,7 +2578,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>223</v>
       </c>
@@ -2597,7 +2613,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>232</v>
       </c>
@@ -2632,7 +2648,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>240</v>
       </c>
@@ -2667,7 +2683,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2702,7 +2718,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>257</v>
       </c>
@@ -2737,7 +2753,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>264</v>
       </c>
@@ -2772,7 +2788,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>257</v>
       </c>
@@ -2807,7 +2823,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>274</v>
       </c>
@@ -2842,7 +2858,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11">
       <c r="A36" t="s">
         <v>282</v>
       </c>
@@ -2877,7 +2893,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>291</v>
       </c>
@@ -2912,7 +2928,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>298</v>
       </c>
@@ -2947,7 +2963,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2982,7 +2998,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>291</v>
       </c>
@@ -3017,7 +3033,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>319</v>
       </c>
@@ -3052,7 +3068,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>326</v>
       </c>
@@ -3087,7 +3103,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>334</v>
       </c>
@@ -3122,7 +3138,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>133</v>
       </c>
@@ -3157,7 +3173,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>348</v>
       </c>
@@ -3192,7 +3208,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11">
       <c r="A46" t="s">
         <v>356</v>
       </c>
@@ -3227,7 +3243,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>364</v>
       </c>
@@ -3262,7 +3278,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>125</v>
       </c>
@@ -3297,7 +3313,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>378</v>
       </c>
@@ -3332,7 +3348,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -3367,7 +3383,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>392</v>
       </c>

</xml_diff>